<commit_message>
Ajout des Script de génération de la base
</commit_message>
<xml_diff>
--- a/representation des tables.xlsx
+++ b/representation des tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taill\Documents\ESIEE\E3FI\BDD\DatabasePizzaProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61FD041-EE3D-40CF-BB93-897A30399339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80C1BA4-3B6B-4856-ACAE-D2F50C9207A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5625" yWindow="-270" windowWidth="28800" windowHeight="11040" xr2:uid="{55B1791C-D3B2-41E0-879F-F2C4C1884ADD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15990" xr2:uid="{55B1791C-D3B2-41E0-879F-F2C4C1884ADD}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="87">
   <si>
     <t>Ingredient</t>
   </si>
@@ -453,13 +453,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -487,6 +490,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -803,10 +812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CDD77AE-9EBC-4B0F-8497-B4D77181B7AE}">
-  <dimension ref="B1:Q34"/>
+  <dimension ref="B1:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y25" sqref="Y25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,25 +834,24 @@
   <sheetData>
     <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="E2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="E2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="11"/>
       <c r="G2" s="10"/>
-      <c r="H2" s="9"/>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="14"/>
     </row>
     <row r="3" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
@@ -861,9 +869,6 @@
       <c r="G3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="J3" s="5" t="s">
         <v>17</v>
       </c>
@@ -896,31 +901,28 @@
       <c r="E4" s="1">
         <v>1</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="2">
         <v>6</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="J4" s="1">
         <v>1</v>
       </c>
-      <c r="K4" s="14">
+      <c r="K4" s="15">
         <v>43996</v>
       </c>
-      <c r="L4" s="14">
+      <c r="L4" s="15">
         <v>43996</v>
       </c>
-      <c r="M4" s="16">
-        <v>1</v>
-      </c>
-      <c r="N4" s="16">
-        <v>1</v>
-      </c>
-      <c r="O4" s="16">
+      <c r="M4" s="17">
+        <v>1</v>
+      </c>
+      <c r="N4" s="17">
+        <v>1</v>
+      </c>
+      <c r="O4" s="17">
         <v>1</v>
       </c>
       <c r="P4" s="2">
@@ -937,31 +939,28 @@
       <c r="E5" s="1">
         <v>2</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="7">
-        <v>6.5</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>31</v>
+      <c r="G5" s="2">
+        <v>7</v>
       </c>
       <c r="J5" s="1">
         <v>2</v>
       </c>
-      <c r="K5" s="14">
+      <c r="K5" s="15">
         <v>43996</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5" s="15">
         <v>43996</v>
       </c>
-      <c r="M5" s="16">
-        <v>1</v>
-      </c>
-      <c r="N5" s="16">
-        <v>2</v>
-      </c>
-      <c r="O5" s="16">
+      <c r="M5" s="17">
+        <v>1</v>
+      </c>
+      <c r="N5" s="17">
+        <v>2</v>
+      </c>
+      <c r="O5" s="17">
         <v>1</v>
       </c>
       <c r="P5" s="2">
@@ -978,31 +977,28 @@
       <c r="E6" s="1">
         <v>3</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="2">
         <v>7</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="J6" s="1">
         <v>3</v>
       </c>
-      <c r="K6" s="14">
+      <c r="K6" s="15">
         <v>43996</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="15">
         <v>43996</v>
       </c>
-      <c r="M6" s="16">
-        <v>1</v>
-      </c>
-      <c r="N6" s="16">
-        <v>3</v>
-      </c>
-      <c r="O6" s="16">
+      <c r="M6" s="17">
+        <v>1</v>
+      </c>
+      <c r="N6" s="17">
+        <v>3</v>
+      </c>
+      <c r="O6" s="17">
         <v>1</v>
       </c>
       <c r="P6" s="2">
@@ -1019,31 +1015,28 @@
       <c r="E7" s="1">
         <v>4</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="2">
         <v>10</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="J7" s="1">
         <v>4</v>
       </c>
-      <c r="K7" s="14">
+      <c r="K7" s="15">
         <v>44027</v>
       </c>
-      <c r="L7" s="14">
+      <c r="L7" s="15">
         <v>44027</v>
       </c>
-      <c r="M7" s="16">
-        <v>1</v>
-      </c>
-      <c r="N7" s="16">
+      <c r="M7" s="17">
+        <v>1</v>
+      </c>
+      <c r="N7" s="17">
         <v>4</v>
       </c>
-      <c r="O7" s="16">
+      <c r="O7" s="17">
         <v>2</v>
       </c>
       <c r="P7" s="2">
@@ -1060,31 +1053,28 @@
       <c r="E8" s="1">
         <v>5</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="7">
-        <v>10.5</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>32</v>
+      <c r="G8" s="2">
+        <v>11</v>
       </c>
       <c r="J8" s="1">
         <v>5</v>
       </c>
-      <c r="K8" s="14">
+      <c r="K8" s="15">
         <v>44027</v>
       </c>
-      <c r="L8" s="14">
+      <c r="L8" s="15">
         <v>44027</v>
       </c>
-      <c r="M8" s="16">
-        <v>1</v>
-      </c>
-      <c r="N8" s="16">
-        <v>1</v>
-      </c>
-      <c r="O8" s="16">
+      <c r="M8" s="17">
+        <v>1</v>
+      </c>
+      <c r="N8" s="17">
+        <v>1</v>
+      </c>
+      <c r="O8" s="17">
         <v>2</v>
       </c>
       <c r="P8" s="2">
@@ -1101,31 +1091,28 @@
       <c r="E9" s="3">
         <v>6</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="4">
         <v>12</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="J9" s="1">
         <v>6</v>
       </c>
-      <c r="K9" s="14">
+      <c r="K9" s="15">
         <v>44027</v>
       </c>
-      <c r="L9" s="14">
+      <c r="L9" s="15">
         <v>44027</v>
       </c>
-      <c r="M9" s="16">
-        <v>1</v>
-      </c>
-      <c r="N9" s="16">
-        <v>2</v>
-      </c>
-      <c r="O9" s="16">
+      <c r="M9" s="17">
+        <v>1</v>
+      </c>
+      <c r="N9" s="17">
+        <v>2</v>
+      </c>
+      <c r="O9" s="17">
         <v>2</v>
       </c>
       <c r="P9" s="2">
@@ -1142,19 +1129,19 @@
       <c r="J10" s="1">
         <v>7</v>
       </c>
-      <c r="K10" s="14">
+      <c r="K10" s="15">
         <v>44032</v>
       </c>
-      <c r="L10" s="14">
+      <c r="L10" s="15">
         <v>44032</v>
       </c>
-      <c r="M10" s="16">
-        <v>2</v>
-      </c>
-      <c r="N10" s="16">
-        <v>3</v>
-      </c>
-      <c r="O10" s="16">
+      <c r="M10" s="17">
+        <v>2</v>
+      </c>
+      <c r="N10" s="17">
+        <v>3</v>
+      </c>
+      <c r="O10" s="17">
         <v>3</v>
       </c>
       <c r="P10" s="2">
@@ -1171,19 +1158,19 @@
       <c r="J11" s="1">
         <v>8</v>
       </c>
-      <c r="K11" s="14">
+      <c r="K11" s="15">
         <v>44033</v>
       </c>
-      <c r="L11" s="14">
+      <c r="L11" s="15">
         <v>44033</v>
       </c>
-      <c r="M11" s="16">
-        <v>3</v>
-      </c>
-      <c r="N11" s="16">
+      <c r="M11" s="17">
+        <v>3</v>
+      </c>
+      <c r="N11" s="17">
         <v>4</v>
       </c>
-      <c r="O11" s="16">
+      <c r="O11" s="17">
         <v>3</v>
       </c>
       <c r="P11" s="2">
@@ -1200,17 +1187,17 @@
       <c r="J12" s="1">
         <v>9</v>
       </c>
-      <c r="K12" s="14">
+      <c r="K12" s="15">
         <v>44035</v>
       </c>
-      <c r="L12" s="14"/>
-      <c r="M12" s="16">
+      <c r="L12" s="15"/>
+      <c r="M12" s="17">
         <v>4</v>
       </c>
-      <c r="N12" s="16">
-        <v>1</v>
-      </c>
-      <c r="O12" s="16">
+      <c r="N12" s="17">
+        <v>1</v>
+      </c>
+      <c r="O12" s="17">
         <v>3</v>
       </c>
       <c r="P12" s="2">
@@ -1227,17 +1214,17 @@
       <c r="J13" s="3">
         <v>10</v>
       </c>
-      <c r="K13" s="15">
+      <c r="K13" s="16">
         <v>44035</v>
       </c>
-      <c r="L13" s="15"/>
-      <c r="M13" s="6">
-        <v>1</v>
-      </c>
-      <c r="N13" s="6">
-        <v>2</v>
-      </c>
-      <c r="O13" s="6">
+      <c r="L13" s="16"/>
+      <c r="M13" s="7">
+        <v>1</v>
+      </c>
+      <c r="N13" s="7">
+        <v>2</v>
+      </c>
+      <c r="O13" s="7">
         <v>1</v>
       </c>
       <c r="P13" s="4">
@@ -1253,30 +1240,31 @@
       </c>
     </row>
     <row r="16" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="8" t="s">
+    <row r="17" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="9"/>
-      <c r="G17" s="8" t="s">
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="10"/>
+      <c r="G17" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="9"/>
-      <c r="M17" s="8" t="s">
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="10"/>
+      <c r="M17" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N17" s="9"/>
-      <c r="P17" s="8" t="s">
+      <c r="N17" s="10"/>
+      <c r="P17" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="Q17" s="9"/>
-    </row>
-    <row r="18" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q17" s="11"/>
+      <c r="R17" s="10"/>
+    </row>
+    <row r="18" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
         <v>21</v>
       </c>
@@ -1316,15 +1304,18 @@
       <c r="Q18" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R18" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>1</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="8" t="s">
         <v>47</v>
       </c>
       <c r="E19" s="2">
@@ -1333,13 +1324,13 @@
       <c r="G19" s="1">
         <v>1</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="H19" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="I19" s="7">
+      <c r="I19" s="8">
         <v>83400</v>
       </c>
-      <c r="J19" s="7" t="s">
+      <c r="J19" s="8" t="s">
         <v>58</v>
       </c>
       <c r="K19" s="2">
@@ -1348,24 +1339,27 @@
       <c r="M19" s="1">
         <v>1</v>
       </c>
-      <c r="N19" s="17">
+      <c r="N19" s="18">
         <v>5.1100000000000003</v>
       </c>
       <c r="P19" s="1">
         <v>1</v>
       </c>
-      <c r="Q19" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q19" s="6">
+        <v>1</v>
+      </c>
+      <c r="R19" s="18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>2</v>
       </c>
       <c r="C20" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="8" t="s">
         <v>52</v>
       </c>
       <c r="E20" s="2">
@@ -1374,13 +1368,13 @@
       <c r="G20" s="1">
         <v>2</v>
       </c>
-      <c r="H20" s="7" t="s">
+      <c r="H20" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="I20" s="7">
+      <c r="I20" s="8">
         <v>77420</v>
       </c>
-      <c r="J20" s="7" t="s">
+      <c r="J20" s="8" t="s">
         <v>59</v>
       </c>
       <c r="K20" s="2">
@@ -1389,24 +1383,27 @@
       <c r="M20" s="1">
         <v>2</v>
       </c>
-      <c r="N20" s="17" t="s">
+      <c r="N20" s="18" t="s">
         <v>82</v>
       </c>
       <c r="P20" s="1">
         <v>1</v>
       </c>
-      <c r="Q20" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q20" s="20">
+        <v>2</v>
+      </c>
+      <c r="R20" s="18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>3</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="17" t="s">
         <v>54</v>
       </c>
       <c r="E21" s="2">
@@ -1415,13 +1412,13 @@
       <c r="G21" s="1">
         <v>3</v>
       </c>
-      <c r="H21" s="7" t="s">
+      <c r="H21" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="I21" s="7">
+      <c r="I21" s="8">
         <v>81200</v>
       </c>
-      <c r="J21" s="16" t="s">
+      <c r="J21" s="17" t="s">
         <v>60</v>
       </c>
       <c r="K21" s="2">
@@ -1430,24 +1427,27 @@
       <c r="M21" s="1">
         <v>3</v>
       </c>
-      <c r="N21" s="17" t="s">
+      <c r="N21" s="18" t="s">
         <v>83</v>
       </c>
       <c r="P21" s="1">
         <v>2</v>
       </c>
-      <c r="Q21" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q21" s="20">
+        <v>3</v>
+      </c>
+      <c r="R21" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <v>4</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="7" t="s">
         <v>53</v>
       </c>
       <c r="E22" s="4">
@@ -1456,13 +1456,13 @@
       <c r="G22" s="3">
         <v>4</v>
       </c>
-      <c r="H22" s="6" t="s">
+      <c r="H22" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="I22" s="6">
+      <c r="I22" s="7">
         <v>83400</v>
       </c>
-      <c r="J22" s="6" t="s">
+      <c r="J22" s="7" t="s">
         <v>61</v>
       </c>
       <c r="K22" s="4">
@@ -1471,99 +1471,120 @@
       <c r="M22" s="1">
         <v>4</v>
       </c>
-      <c r="N22" s="17" t="s">
+      <c r="N22" s="18" t="s">
         <v>84</v>
       </c>
       <c r="P22" s="1">
         <v>4</v>
       </c>
-      <c r="Q22" s="17">
+      <c r="Q22" s="20">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R22" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M23" s="1">
         <v>5</v>
       </c>
-      <c r="N23" s="17" t="s">
+      <c r="N23" s="18" t="s">
         <v>85</v>
       </c>
       <c r="P23" s="1">
         <v>6</v>
       </c>
-      <c r="Q23" s="17">
+      <c r="Q23" s="20">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R23" s="18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M24" s="3">
         <v>6</v>
       </c>
-      <c r="N24" s="18" t="s">
+      <c r="N24" s="19" t="s">
         <v>86</v>
       </c>
       <c r="P24" s="1">
         <v>8</v>
       </c>
-      <c r="Q24" s="17">
+      <c r="Q24" s="20">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R24" s="18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="P25" s="1">
         <v>1</v>
       </c>
-      <c r="Q25" s="17">
+      <c r="Q25" s="20">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R25" s="18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="P26" s="1">
         <v>3</v>
       </c>
-      <c r="Q26" s="17">
+      <c r="Q26" s="20">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R26" s="18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P27" s="1">
         <v>4</v>
       </c>
-      <c r="Q27" s="17">
+      <c r="Q27" s="20">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="8" t="s">
+      <c r="R27" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="9"/>
-      <c r="H28" s="8" t="s">
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="10"/>
+      <c r="H28" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="I28" s="10"/>
-      <c r="J28" s="9"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="10"/>
       <c r="P28" s="3">
         <v>9</v>
       </c>
-      <c r="Q28" s="18">
+      <c r="Q28" s="21">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R28" s="19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E29" s="8" t="s">
         <v>64</v>
       </c>
       <c r="F29" s="2" t="s">
@@ -1572,24 +1593,24 @@
       <c r="H29" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I29" s="7" t="s">
+      <c r="I29" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>1</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="8">
         <v>639</v>
       </c>
       <c r="F30" s="2">
@@ -1598,24 +1619,24 @@
       <c r="H30" s="1">
         <v>1</v>
       </c>
-      <c r="I30" s="7" t="s">
+      <c r="I30" s="8" t="s">
         <v>74</v>
       </c>
       <c r="J30" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" s="1">
         <v>2</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="8">
         <v>100</v>
       </c>
       <c r="F31" s="2">
@@ -1624,24 +1645,24 @@
       <c r="H31" s="1">
         <v>2</v>
       </c>
-      <c r="I31" s="7" t="s">
+      <c r="I31" s="8" t="s">
         <v>75</v>
       </c>
       <c r="J31" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="1">
         <v>3</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C32" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="D32" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="8">
         <v>25</v>
       </c>
       <c r="F32" s="2">
@@ -1650,7 +1671,7 @@
       <c r="H32" s="3">
         <v>3</v>
       </c>
-      <c r="I32" s="6" t="s">
+      <c r="I32" s="7" t="s">
         <v>76</v>
       </c>
       <c r="J32" s="4" t="s">
@@ -1661,13 +1682,13 @@
       <c r="B33" s="3">
         <v>4</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E33" s="7">
         <v>10</v>
       </c>
       <c r="F33" s="4">
@@ -1675,23 +1696,23 @@
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="B28:F28"/>
     <mergeCell ref="M17:N17"/>
-    <mergeCell ref="P17:Q17"/>
     <mergeCell ref="H28:J28"/>
+    <mergeCell ref="P17:R17"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="E2:H2"/>
     <mergeCell ref="J2:P2"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="G17:K17"/>
+    <mergeCell ref="E2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>